<commit_message>
Se agrega Estados de Acción a la planilla de tablas
</commit_message>
<xml_diff>
--- a/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
+++ b/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="485">
   <si>
     <t>TIPO DE INCIDENCIA</t>
   </si>
@@ -1464,6 +1464,18 @@
   </si>
   <si>
     <t>Padre Hurtado</t>
+  </si>
+  <si>
+    <t>ESTADOS DE ACCIÓN</t>
+  </si>
+  <si>
+    <t>EstadosAccion</t>
+  </si>
+  <si>
+    <t>Incumple con lo dispuesto</t>
+  </si>
+  <si>
+    <t>Cumple con lo dispuesto</t>
   </si>
 </sst>
 </file>
@@ -1857,7 +1869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1865,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2390,7 +2402,7 @@
         <v>INSERT INTO Roles VALUES (1, 'Coordinador', 1)</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>INSERT INTO Roles VALUES (2, 'Director Responsable', 1)</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -2424,6 +2436,32 @@
       <c r="G34" t="str">
         <f t="shared" si="2"/>
         <v>INSERT INTO Roles VALUES (3, 'Representante Alta Dirección', 1)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>481</v>
+      </c>
+      <c r="B36" t="s">
+        <v>482</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>482</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega a la planilla de tablas y comandos sql el script de estadosaccion. Se exporta el script EstadosAccion.sql
</commit_message>
<xml_diff>
--- a/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
+++ b/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
@@ -1869,7 +1869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,7 +1880,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="G37" sqref="G36:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" ref="G24:G34" si="2">CONCATENATE("INSERT INTO ",B24," VALUES (",C24,", '",D24,"', ",IF(E24=1,1,0),")")</f>
+        <f t="shared" ref="G24:G37" si="2">CONCATENATE("INSERT INTO ",B24," VALUES (",C24,", '",D24,"', ",IF(E24=1,1,0),")")</f>
         <v>INSERT INTO Tratamientos VALUES (2, 'Desecho', 1)</v>
       </c>
     </row>
@@ -2452,6 +2452,13 @@
       <c r="D36" t="s">
         <v>484</v>
       </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO EstadosAccion VALUES (1, 'Cumple con lo dispuesto', 1)</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -2462,6 +2469,13 @@
       </c>
       <c r="D37" t="s">
         <v>483</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO EstadosAccion VALUES (2, 'Incumple con lo dispuesto', 1)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualizan cambios solicitados por profesor
</commit_message>
<xml_diff>
--- a/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
+++ b/Otros/Documentación Componentes Tablas y Comandos SQL.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="487">
   <si>
     <t>TIPO DE INCIDENCIA</t>
   </si>
@@ -1481,6 +1481,12 @@
   </si>
   <si>
     <t>En espera de revisión</t>
+  </si>
+  <si>
+    <t>Esp.</t>
+  </si>
+  <si>
+    <t>Dias</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,6 +1921,9 @@
       <c r="E1" t="s">
         <v>16</v>
       </c>
+      <c r="F1" t="s">
+        <v>485</v>
+      </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
@@ -2237,7 +2246,11 @@
         <v>INSERT INTO EstadosIncidencia VALUES (6, 'Finalizada', 1)</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="9" t="s">
+        <v>486</v>
+      </c>
+    </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
@@ -2254,9 +2267,12 @@
       <c r="E23">
         <v>1</v>
       </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
       <c r="G23" t="str">
-        <f>CONCATENATE("INSERT INTO ",B23," VALUES (",C23,", '",D23,"', ",IF(E23=1,1,0),")")</f>
-        <v>INSERT INTO Tratamientos VALUES (1, 'Concesión', 1)</v>
+        <f>CONCATENATE("INSERT INTO ",B23," VALUES (",C23,", '",D23,"', ",IF(E23=1,1,0),", ",F23,")")</f>
+        <v>INSERT INTO Tratamientos VALUES (1, 'Concesión', 1, 2)</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2272,9 +2288,12 @@
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
       <c r="G24" t="str">
-        <f t="shared" ref="G24:G37" si="2">CONCATENATE("INSERT INTO ",B24," VALUES (",C24,", '",D24,"', ",IF(E24=1,1,0),")")</f>
-        <v>INSERT INTO Tratamientos VALUES (2, 'Desecho', 1)</v>
+        <f t="shared" ref="G24:G30" si="2">CONCATENATE("INSERT INTO ",B24," VALUES (",C24,", '",D24,"', ",IF(E24=1,1,0),", ",F24,")")</f>
+        <v>INSERT INTO Tratamientos VALUES (2, 'Desecho', 1, 2)</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2290,9 +2309,12 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
       <c r="G25" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (3, 'Liberar', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (3, 'Liberar', 1, 3)</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2308,9 +2330,12 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
       <c r="G26" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (4, 'Permiso de Desviación', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (4, 'Permiso de Desviación', 1, 2)</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2326,9 +2351,12 @@
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
       <c r="G27" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (5, 'Reclasificación', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (5, 'Reclasificación', 1, 4)</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,9 +2372,12 @@
       <c r="E28">
         <v>1</v>
       </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (6, 'Reparación', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (6, 'Reparación', 1, 5)</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2362,9 +2393,12 @@
       <c r="E29">
         <v>1</v>
       </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
       <c r="G29" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (7, 'Reproceso', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (7, 'Reproceso', 1, 2)</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2380,9 +2414,12 @@
       <c r="E30">
         <v>1</v>
       </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
       <c r="G30" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO Tratamientos VALUES (8, 'Verificación', 1)</v>
+        <v>INSERT INTO Tratamientos VALUES (8, 'Verificación', 1, 3)</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2403,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G24:G37" si="3">CONCATENATE("INSERT INTO ",B32," VALUES (",C32,", '",D32,"', ",IF(E32=1,1,0),")")</f>
         <v>INSERT INTO Roles VALUES (1, 'Coordinador', 1)</v>
       </c>
     </row>
@@ -2421,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Roles VALUES (2, 'Director Responsable', 1)</v>
       </c>
     </row>
@@ -2439,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Roles VALUES (3, 'Representante Alta Dirección', 1)</v>
       </c>
     </row>
@@ -2461,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO EstadosAccion VALUES (1, 'Cumple con lo dispuesto', 1)</v>
       </c>
     </row>
@@ -2479,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO EstadosAccion VALUES (2, 'Incumple con lo dispuesto', 1)</v>
       </c>
     </row>

</xml_diff>